<commit_message>
Thats the Fish Harvest data complete
</commit_message>
<xml_diff>
--- a/Data_Raw/Benefish 3 Excel files/Employment_FFA tuna employment_edAM.xlsx
+++ b/Data_Raw/Benefish 3 Excel files/Employment_FFA tuna employment_edAM.xlsx
@@ -1281,21 +1281,12 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4ED6A4C4-E5CA-437B-8E5C-EC17688233A9}" diskRevisions="1" revisionId="6" version="2">
-  <header guid="{241CC5FE-3F5D-42D4-B461-32C19DA279EB}" dateTime="2016-05-26T14:03:57" maxSheetId="2" userName="Anne Moorhead" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
   <header guid="{4ED6A4C4-E5CA-437B-8E5C-EC17688233A9}" dateTime="2016-05-26T14:04:53" maxSheetId="2" userName="Anne Moorhead" r:id="rId2" minRId="1" maxRId="6">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>